<commit_message>
upload analysis from 20200306
</commit_message>
<xml_diff>
--- a/code/processing/growth_curves_plate_reader/20200306_r1_O2_mCherry_NiCl2/20200306_plate_layout.xlsx
+++ b/code/processing/growth_curves_plate_reader/20200306_r1_O2_mCherry_NiCl2/20200306_plate_layout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/razo/Documents/PhD/evo_mwc/code/processing/growth_curves_plate_reader/202003056_r1_O2_mCherry_NiCl2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/razo/Documents/PhD/evo_mwc/code/processing/growth_curves_plate_reader/20200306_r1_O2_mCherry_NiCl2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="19740" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="strain" sheetId="1" r:id="rId1"/>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,34 +942,34 @@
         <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L7" t="s">
         <v>97</v>
@@ -1983,7 +1983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>

</xml_diff>